<commit_message>
data change auto refresh added
</commit_message>
<xml_diff>
--- a/backend/media/PRO  INFO (6).xlsx
+++ b/backend/media/PRO  INFO (6).xlsx
@@ -137,12 +137,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -166,120 +166,111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.9514170040486"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.4858299595142"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1955</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1955</v>
+        <v>2004</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>2004</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:T1"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>